<commit_message>
added some missing countries
</commit_message>
<xml_diff>
--- a/data/lang_tools/country_to_lang/cia_factbook_data.xlsx
+++ b/data/lang_tools/country_to_lang/cia_factbook_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14320" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="14320" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CIA Orig" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1171" uniqueCount="1125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="1152">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -3395,6 +3395,87 @@
   </si>
   <si>
     <t>eng": 8, "lug": 14</t>
+  </si>
+  <si>
+    <t>"PG"</t>
+  </si>
+  <si>
+    <t>"BS"</t>
+  </si>
+  <si>
+    <t>"BZ"</t>
+  </si>
+  <si>
+    <t>"GD"</t>
+  </si>
+  <si>
+    <t>"Papua New Guinea"</t>
+  </si>
+  <si>
+    <t>"Bahamas, The"</t>
+  </si>
+  <si>
+    <t>"Belize"</t>
+  </si>
+  <si>
+    <t>"Grenada"</t>
+  </si>
+  <si>
+    <t>eng": 2, "tpi":1.8</t>
+  </si>
+  <si>
+    <t>eng":41, "spa":32</t>
+  </si>
+  <si>
+    <t>eng":82, "fra":2</t>
+  </si>
+  <si>
+    <t>"FJ"</t>
+  </si>
+  <si>
+    <t>"Fiji"</t>
+  </si>
+  <si>
+    <t>hif":45.3, "fij":39.3</t>
+  </si>
+  <si>
+    <t>"KI"</t>
+  </si>
+  <si>
+    <t>"KM"</t>
+  </si>
+  <si>
+    <t>"DM"</t>
+  </si>
+  <si>
+    <t>"VC"</t>
+  </si>
+  <si>
+    <t>"AG"</t>
+  </si>
+  <si>
+    <t>"ST"</t>
+  </si>
+  <si>
+    <t>"Kiribati"</t>
+  </si>
+  <si>
+    <t>"Comoros"</t>
+  </si>
+  <si>
+    <t>"Dominica"</t>
+  </si>
+  <si>
+    <t>"Saint Vincent and the Grenadines"</t>
+  </si>
+  <si>
+    <t>"Antigua and Barbuda"</t>
+  </si>
+  <si>
+    <t>"Sao Tome and Principe"</t>
+  </si>
+  <si>
+    <t>gil":62.6</t>
   </si>
 </sst>
 </file>
@@ -3448,8 +3529,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="129">
+  <cellStyleXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3584,7 +3667,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="129">
+  <cellStyles count="131">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3649,6 +3732,7 @@
     <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3713,6 +3797,7 @@
     <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6208,10 +6293,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J195"/>
+  <dimension ref="A1:J206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
-      <selection activeCell="C183" sqref="C183"/>
+    <sheetView tabSelected="1" topLeftCell="I194" workbookViewId="0">
+      <selection activeCell="J204" sqref="J204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11468,20 +11553,302 @@
         <v>724</v>
       </c>
       <c r="G195" s="2" t="str">
-        <f t="shared" ref="G195" si="12" xml:space="preserve"> A195 &amp; ": {"</f>
+        <f t="shared" ref="G195:G206" si="12" xml:space="preserve"> A195 &amp; ": {"</f>
         <v>"ZW": {</v>
       </c>
       <c r="H195" t="str">
-        <f t="shared" ref="H195" si="13">"""name"": " &amp;B195&amp;", ""langs"": {"</f>
+        <f t="shared" ref="H195:H206" si="13">"""name"": " &amp;B195&amp;", ""langs"": {"</f>
         <v>"name": "Zimbabwe", "langs": {</v>
       </c>
       <c r="I195" t="str">
-        <f t="shared" ref="I195" si="14">"""" &amp; C195 &amp; "}},"</f>
+        <f t="shared" ref="I195:I206" si="14">"""" &amp; C195 &amp; "}},"</f>
         <v>"sna": 70, "nde":20, "eng": 2.5}},</v>
       </c>
       <c r="J195" t="str">
-        <f t="shared" ref="J195" si="15">G195&amp;H195&amp;I195</f>
+        <f t="shared" ref="J195:J206" si="15">G195&amp;H195&amp;I195</f>
         <v>"ZW": {"name": "Zimbabwe", "langs": {"sna": 70, "nde":20, "eng": 2.5}},</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10" ht="16">
+      <c r="A196" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B196" t="s">
+        <v>1129</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>1133</v>
+      </c>
+      <c r="G196" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>"PG": {</v>
+      </c>
+      <c r="H196" t="str">
+        <f t="shared" si="13"/>
+        <v>"name": "Papua New Guinea", "langs": {</v>
+      </c>
+      <c r="I196" t="str">
+        <f t="shared" si="14"/>
+        <v>"eng": 2, "tpi":1.8}},</v>
+      </c>
+      <c r="J196" t="str">
+        <f t="shared" si="15"/>
+        <v>"PG": {"name": "Papua New Guinea", "langs": {"eng": 2, "tpi":1.8}},</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10" ht="16">
+      <c r="A197" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B197" t="s">
+        <v>1130</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="G197" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>"BS": {</v>
+      </c>
+      <c r="H197" t="str">
+        <f t="shared" si="13"/>
+        <v>"name": "Bahamas, The", "langs": {</v>
+      </c>
+      <c r="I197" t="str">
+        <f t="shared" si="14"/>
+        <v>"eng":100}},</v>
+      </c>
+      <c r="J197" t="str">
+        <f t="shared" si="15"/>
+        <v>"BS": {"name": "Bahamas, The", "langs": {"eng":100}},</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10" ht="16">
+      <c r="A198" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B198" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>1134</v>
+      </c>
+      <c r="G198" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>"BZ": {</v>
+      </c>
+      <c r="H198" t="str">
+        <f t="shared" si="13"/>
+        <v>"name": "Belize", "langs": {</v>
+      </c>
+      <c r="I198" t="str">
+        <f t="shared" si="14"/>
+        <v>"eng":41, "spa":32}},</v>
+      </c>
+      <c r="J198" t="str">
+        <f t="shared" si="15"/>
+        <v>"BZ": {"name": "Belize", "langs": {"eng":41, "spa":32}},</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10" ht="16">
+      <c r="A199" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B199" t="s">
+        <v>1132</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>1135</v>
+      </c>
+      <c r="G199" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>"GD": {</v>
+      </c>
+      <c r="H199" t="str">
+        <f t="shared" si="13"/>
+        <v>"name": "Grenada", "langs": {</v>
+      </c>
+      <c r="I199" t="str">
+        <f t="shared" si="14"/>
+        <v>"eng":82, "fra":2}},</v>
+      </c>
+      <c r="J199" t="str">
+        <f t="shared" si="15"/>
+        <v>"GD": {"name": "Grenada", "langs": {"eng":82, "fra":2}},</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10" ht="16">
+      <c r="A200" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B200" t="s">
+        <v>1137</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>1138</v>
+      </c>
+      <c r="G200" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>"FJ": {</v>
+      </c>
+      <c r="H200" t="str">
+        <f t="shared" si="13"/>
+        <v>"name": "Fiji", "langs": {</v>
+      </c>
+      <c r="I200" t="str">
+        <f t="shared" si="14"/>
+        <v>"hif":45.3, "fij":39.3}},</v>
+      </c>
+      <c r="J200" t="str">
+        <f t="shared" si="15"/>
+        <v>"FJ": {"name": "Fiji", "langs": {"hif":45.3, "fij":39.3}},</v>
+      </c>
+    </row>
+    <row r="201" spans="1:10" ht="16">
+      <c r="A201" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B201" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>1151</v>
+      </c>
+      <c r="G201" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>"KI": {</v>
+      </c>
+      <c r="H201" t="str">
+        <f t="shared" si="13"/>
+        <v>"name": "Kiribati", "langs": {</v>
+      </c>
+      <c r="I201" t="str">
+        <f t="shared" si="14"/>
+        <v>"gil":62.6}},</v>
+      </c>
+      <c r="J201" t="str">
+        <f t="shared" si="15"/>
+        <v>"KI": {"name": "Kiribati", "langs": {"gil":62.6}},</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10" ht="16">
+      <c r="A202" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B202" t="s">
+        <v>1146</v>
+      </c>
+      <c r="G202" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>"KM": {</v>
+      </c>
+      <c r="H202" t="str">
+        <f t="shared" si="13"/>
+        <v>"name": "Comoros", "langs": {</v>
+      </c>
+      <c r="I202" t="str">
+        <f t="shared" si="14"/>
+        <v>"}},</v>
+      </c>
+      <c r="J202" t="str">
+        <f t="shared" si="15"/>
+        <v>"KM": {"name": "Comoros", "langs": {"}},</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10" ht="16">
+      <c r="A203" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B203" t="s">
+        <v>1147</v>
+      </c>
+      <c r="G203" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>"DM": {</v>
+      </c>
+      <c r="H203" t="str">
+        <f t="shared" si="13"/>
+        <v>"name": "Dominica", "langs": {</v>
+      </c>
+      <c r="I203" t="str">
+        <f t="shared" si="14"/>
+        <v>"}},</v>
+      </c>
+      <c r="J203" t="str">
+        <f t="shared" si="15"/>
+        <v>"DM": {"name": "Dominica", "langs": {"}},</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10" ht="16">
+      <c r="A204" t="s">
+        <v>1142</v>
+      </c>
+      <c r="B204" t="s">
+        <v>1148</v>
+      </c>
+      <c r="G204" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>"VC": {</v>
+      </c>
+      <c r="H204" t="str">
+        <f t="shared" si="13"/>
+        <v>"name": "Saint Vincent and the Grenadines", "langs": {</v>
+      </c>
+      <c r="I204" t="str">
+        <f t="shared" si="14"/>
+        <v>"}},</v>
+      </c>
+      <c r="J204" t="str">
+        <f t="shared" si="15"/>
+        <v>"VC": {"name": "Saint Vincent and the Grenadines", "langs": {"}},</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10" ht="16">
+      <c r="A205" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B205" t="s">
+        <v>1149</v>
+      </c>
+      <c r="G205" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>"AG": {</v>
+      </c>
+      <c r="H205" t="str">
+        <f t="shared" si="13"/>
+        <v>"name": "Antigua and Barbuda", "langs": {</v>
+      </c>
+      <c r="I205" t="str">
+        <f t="shared" si="14"/>
+        <v>"}},</v>
+      </c>
+      <c r="J205" t="str">
+        <f t="shared" si="15"/>
+        <v>"AG": {"name": "Antigua and Barbuda", "langs": {"}},</v>
+      </c>
+    </row>
+    <row r="206" spans="1:10" ht="16">
+      <c r="A206" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B206" t="s">
+        <v>1150</v>
+      </c>
+      <c r="G206" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>"ST": {</v>
+      </c>
+      <c r="H206" t="str">
+        <f t="shared" si="13"/>
+        <v>"name": "Sao Tome and Principe", "langs": {</v>
+      </c>
+      <c r="I206" t="str">
+        <f t="shared" si="14"/>
+        <v>"}},</v>
+      </c>
+      <c r="J206" t="str">
+        <f t="shared" si="15"/>
+        <v>"ST": {"name": "Sao Tome and Principe", "langs": {"}},</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates lang shares by country
</commit_message>
<xml_diff>
--- a/data/lang_tools/country_to_lang/cia_factbook_data.xlsx
+++ b/data/lang_tools/country_to_lang/cia_factbook_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="1152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="1157">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -3476,6 +3476,21 @@
   </si>
   <si>
     <t>gil":62.6</t>
+  </si>
+  <si>
+    <t>"Anc. Greece"</t>
+  </si>
+  <si>
+    <t>"Rome"</t>
+  </si>
+  <si>
+    <t>"Arab World"</t>
+  </si>
+  <si>
+    <t>lat":100</t>
+  </si>
+  <si>
+    <t>grc":100</t>
   </si>
 </sst>
 </file>
@@ -3529,8 +3544,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="131">
+  <cellStyleXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3667,7 +3688,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="131">
+  <cellStyles count="137">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3733,6 +3754,9 @@
     <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3798,6 +3822,9 @@
     <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6293,10 +6320,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J206"/>
+  <dimension ref="A1:J209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I194" workbookViewId="0">
-      <selection activeCell="J204" sqref="J204"/>
+    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
+      <selection activeCell="B208" sqref="B208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11851,6 +11878,87 @@
         <v>"ST": {"name": "Sao Tome and Principe", "langs": {"}},</v>
       </c>
     </row>
+    <row r="207" spans="1:10" ht="16">
+      <c r="A207" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B207" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="G207" s="2" t="str">
+        <f t="shared" ref="G207:G209" si="16" xml:space="preserve"> A207 &amp; ": {"</f>
+        <v>"Arab World": {</v>
+      </c>
+      <c r="H207" t="str">
+        <f t="shared" ref="H207:H209" si="17">"""name"": " &amp;B207&amp;", ""langs"": {"</f>
+        <v>"name": "Arab World", "langs": {</v>
+      </c>
+      <c r="I207" t="str">
+        <f t="shared" ref="I207:I209" si="18">"""" &amp; C207 &amp; "}},"</f>
+        <v>"ara":100}},</v>
+      </c>
+      <c r="J207" t="str">
+        <f t="shared" ref="J207:J209" si="19">G207&amp;H207&amp;I207</f>
+        <v>"Arab World": {"name": "Arab World", "langs": {"ara":100}},</v>
+      </c>
+    </row>
+    <row r="208" spans="1:10" ht="16">
+      <c r="A208" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B208" t="s">
+        <v>1153</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>1155</v>
+      </c>
+      <c r="G208" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>"Rome": {</v>
+      </c>
+      <c r="H208" t="str">
+        <f t="shared" si="17"/>
+        <v>"name": "Rome", "langs": {</v>
+      </c>
+      <c r="I208" t="str">
+        <f t="shared" si="18"/>
+        <v>"lat":100}},</v>
+      </c>
+      <c r="J208" t="str">
+        <f t="shared" si="19"/>
+        <v>"Rome": {"name": "Rome", "langs": {"lat":100}},</v>
+      </c>
+    </row>
+    <row r="209" spans="1:10" ht="16">
+      <c r="A209" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B209" t="s">
+        <v>1152</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>1156</v>
+      </c>
+      <c r="G209" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>"Anc. Greece": {</v>
+      </c>
+      <c r="H209" t="str">
+        <f t="shared" si="17"/>
+        <v>"name": "Anc. Greece", "langs": {</v>
+      </c>
+      <c r="I209" t="str">
+        <f t="shared" si="18"/>
+        <v>"grc":100}},</v>
+      </c>
+      <c r="J209" t="str">
+        <f t="shared" si="19"/>
+        <v>"Anc. Greece": {"name": "Anc. Greece", "langs": {"grc":100}},</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>